<commit_message>
Script with corrected protein ladder
</commit_message>
<xml_diff>
--- a/project/Figuring out molecular weight.xlsx
+++ b/project/Figuring out molecular weight.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/492891258891699e/Documents/uni/Uni_Work/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{BCD7BC61-015B-43A5-A8CF-9ED560271D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB884FDA-7063-4708-9413-90529CEABCDB}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{BCD7BC61-015B-43A5-A8CF-9ED560271D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12802669-FBB4-4783-B5B2-2D805BD5B91A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2EA3EDEE-FE5D-443D-B145-482D0D79BC1B}"/>
   </bookViews>
@@ -94,6 +94,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1044B53F-0F6C-49CA-A5C0-4198A7883AA7}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,7 +443,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>6.74</v>
+        <v>7.27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -447,7 +451,7 @@
         <v>15</v>
       </c>
       <c r="B3">
-        <v>5.56</v>
+        <v>6.51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -455,7 +459,7 @@
         <v>20</v>
       </c>
       <c r="B4">
-        <v>5.01</v>
+        <v>5.29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -463,7 +467,7 @@
         <v>25</v>
       </c>
       <c r="B5">
-        <v>4.21</v>
+        <v>4.7699999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -471,7 +475,7 @@
         <v>37</v>
       </c>
       <c r="B6">
-        <v>3.38</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -479,31 +483,39 @@
         <v>50</v>
       </c>
       <c r="B7">
-        <v>2.78</v>
+        <v>3.33</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="B8">
-        <v>2.15</v>
+        <v>2.54</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="B9">
-        <v>1.27</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
+        <v>150</v>
+      </c>
+      <c r="B10">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>250</v>
       </c>
-      <c r="B10">
-        <v>0.56999999999999995</v>
+      <c r="B11">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>